<commit_message>
sql attendance marking, yet new 2 be done
</commit_message>
<xml_diff>
--- a/python/CVPROJECT.xlsx
+++ b/python/CVPROJECT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\captsoneFiles\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B1A495-196E-48F7-9BC1-27334711EB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56485ABB-1057-4AE6-BDF6-D9BFF4279EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>HussainArsiwala</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Aditya</t>
+  </si>
+  <si>
+    <t>B129</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +445,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>